<commit_message>
hand edit to the Excel (which is a copy-laste from the PDF)
</commit_message>
<xml_diff>
--- a/DAC_listed_countries.xlsx
+++ b/DAC_listed_countries.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/riinuots/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/riinuots/Dropbox/RStudio/DAC_listed_countries/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="500" yWindow="460" windowWidth="14160" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="500" yWindow="460" windowWidth="16120" windowHeight="17680" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
   <si>
     <t xml:space="preserve">Bhutan </t>
   </si>
@@ -197,9 +197,6 @@
     <t xml:space="preserve">Gabon </t>
   </si>
   <si>
-    <t>Grenada Iran</t>
-  </si>
-  <si>
     <t xml:space="preserve">Malaysia </t>
   </si>
   <si>
@@ -471,6 +468,12 @@
   </si>
   <si>
     <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Grenada</t>
+  </si>
+  <si>
+    <t>Iran</t>
   </si>
 </sst>
 </file>
@@ -797,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -812,16 +815,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>70</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -887,12 +890,12 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D9" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>25</v>
@@ -900,7 +903,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>42</v>
@@ -908,10 +911,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -919,7 +922,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>43</v>
@@ -956,7 +959,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C18" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -964,7 +967,7 @@
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>47</v>
@@ -977,10 +980,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -988,12 +991,12 @@
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>48</v>
@@ -1001,7 +1004,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>30</v>
@@ -1009,7 +1012,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>49</v>
@@ -1020,12 +1023,12 @@
         <v>5</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>50</v>
@@ -1033,21 +1036,21 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1055,15 +1058,15 @@
         <v>6</v>
       </c>
       <c r="D30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C31" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1071,7 +1074,7 @@
         <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>51</v>
@@ -1079,12 +1082,12 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>32</v>
@@ -1095,7 +1098,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>53</v>
@@ -1103,7 +1106,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>33</v>
@@ -1114,7 +1117,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>34</v>
@@ -1123,7 +1126,7 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>55</v>
@@ -1132,65 +1135,65 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>56</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1199,18 +1202,18 @@
         <v>36</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
+      <c r="D47" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C48" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>57</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1218,97 +1221,95 @@
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>118</v>
+        <v>117</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C50" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D50" s="1" t="s">
-        <v>131</v>
-      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D51" t="s">
-        <v>132</v>
+        <v>91</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D52" s="1" t="s">
-        <v>58</v>
+      <c r="D52" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="D53" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C54" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>59</v>
-      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D56" s="1" t="s">
-        <v>133</v>
+      <c r="D55" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D59" t="s">
-        <v>136</v>
+        <v>95</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>137</v>
+        <v>96</v>
+      </c>
+      <c r="D60" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1318,108 +1319,117 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="D63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>101</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>60</v>
+        <v>100</v>
+      </c>
+      <c r="D64" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>61</v>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D67" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>62</v>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D69" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>63</v>
+        <v>101</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D71" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D74" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D75" s="1" t="s">
-        <v>65</v>
+        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D76" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D77" s="1" t="s">
-        <v>144</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D78" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D79" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D80" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D81" s="1" t="s">
-        <v>67</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D82" s="1" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>